<commit_message>
AJUSTE: archivo y enlace
</commit_message>
<xml_diff>
--- a/public/uploads/files/libro_productos_import.xlsx
+++ b/public/uploads/files/libro_productos_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\alpinav2\public\uploads\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,9 +29,6 @@
     <t>Referencia (Tanto para productos como atributos)</t>
   </si>
   <si>
-    <t>Precio( se definira como precio base del producto o atributo)</t>
-  </si>
-  <si>
     <t>PUM</t>
   </si>
   <si>
@@ -45,6 +42,9 @@
   </si>
   <si>
     <t>Gramo a $35,6 pesos</t>
+  </si>
+  <si>
+    <t>Precio se definira como el precio del rol y ciudad</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,10 +395,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -409,7 +409,7 @@
         <v>9999</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -420,7 +420,7 @@
         <v>9999</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -431,7 +431,7 @@
         <v>9999</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -442,8 +442,11 @@
         <v>9999</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>

</xml_diff>

<commit_message>
Ajuste de pum en carga de precio base y precio por rol
</commit_message>
<xml_diff>
--- a/public/uploads/files/libro_productos_import.xlsx
+++ b/public/uploads/files/libro_productos_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\alpina\public\uploads\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,24 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Referencia (Tanto para productos como atributos)</t>
-  </si>
-  <si>
-    <t>PUM</t>
-  </si>
-  <si>
-    <t>Gramo a $45,6 pesos</t>
-  </si>
-  <si>
-    <t>Gramo a $15,6 pesos</t>
-  </si>
-  <si>
-    <t>Gramo a $25,6 pesos</t>
-  </si>
-  <si>
-    <t>Gramo a $35,6 pesos</t>
   </si>
   <si>
     <t>Precio se definira como el precio del rol y ciudad</t>
@@ -381,101 +366,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>7702001100095</v>
       </c>
       <c r="B2">
         <v>9999</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>7702001101498</v>
       </c>
       <c r="B3">
         <v>9999</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>7702001101573</v>
       </c>
       <c r="B4">
         <v>9999</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>7702001102730</v>
       </c>
       <c r="B5">
         <v>9999</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>